<commit_message>
Minor improvements to the measurement template
</commit_message>
<xml_diff>
--- a/StateOfPractice/Ao-Notes/MedicalImaging_Combined_MeasurementTemplate_EmpiricalMeasures.xlsx
+++ b/StateOfPractice/Ao-Notes/MedicalImaging_Combined_MeasurementTemplate_EmpiricalMeasures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sync\Projs\AIMSS\StateOfPractice\Ao-Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51149839-8435-4403-B67C-6F6641437167}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C28EBB6-378F-4DBE-9D06-CF93E413984B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="212">
   <si>
     <t>Metrics &amp; Description</t>
   </si>
@@ -201,9 +201,6 @@
     <t>({Windows, Linux, OS X, Android, other* }) *given via string</t>
   </si>
   <si>
-    <t>How many software packages need to be installed before or during installation?</t>
-  </si>
-  <si>
     <t>Are required package versions listed?</t>
   </si>
   <si>
@@ -364,9 +361,6 @@
   </si>
   <si>
     <t xml:space="preserve">Explicit identification of a coding standard? </t>
-  </si>
-  <si>
-    <t>({yes∗, no, n/a})</t>
   </si>
   <si>
     <t xml:space="preserve">Are the code identifiers consistent, distinctive, and meaningful? </t>
@@ -735,6 +729,15 @@
   </si>
   <si>
     <t>({number, n/a})</t>
+  </si>
+  <si>
+    <t>How many extra software packages need to be installed before or during installation?</t>
+  </si>
+  <si>
+    <t>({yes, no∗ , unclear})</t>
+  </si>
+  <si>
+    <t>({yes∗, no, unclear})</t>
   </si>
 </sst>
 </file>
@@ -776,20 +779,15 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -847,29 +845,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -921,13 +903,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="注释" xfId="3" builtinId="10"/>
     <cellStyle name="百分比" xfId="2" builtinId="5"/>
     <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
@@ -1244,8 +1222,8 @@
   <dimension ref="A1:AMJ125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1287,13 +1265,13 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:1024" x14ac:dyDescent="0.2">
@@ -1304,13 +1282,13 @@
         <v>7</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:1024" ht="102" x14ac:dyDescent="0.2">
@@ -1321,13 +1299,13 @@
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:1024" ht="63.75" x14ac:dyDescent="0.2">
@@ -1338,13 +1316,13 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:1024" ht="38.25" x14ac:dyDescent="0.2">
@@ -1372,13 +1350,13 @@
         <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
@@ -1397,7 +1375,7 @@
         <v>stars: 91, forks:27, watching: 22</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:1024" s="19" customFormat="1" x14ac:dyDescent="0.2">
@@ -1442,13 +1420,13 @@
         <v>21</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:1024" ht="38.25" x14ac:dyDescent="0.2">
@@ -1459,13 +1437,13 @@
         <v>23</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
@@ -1476,13 +1454,13 @@
         <v>25</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:1024" ht="63.75" x14ac:dyDescent="0.2">
@@ -1493,13 +1471,13 @@
         <v>27</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
@@ -1510,13 +1488,13 @@
         <v>29</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:1024" ht="38.25" x14ac:dyDescent="0.2">
@@ -1545,13 +1523,13 @@
         <v>33</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
@@ -1562,13 +1540,13 @@
         <v>35</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="20" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
@@ -1579,13 +1557,13 @@
         <v>37</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:1024" ht="75.400000000000006" customHeight="1" x14ac:dyDescent="0.2">
@@ -1610,13 +1588,13 @@
         <v>41</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:1024" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -1627,13 +1605,13 @@
         <v>43</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
@@ -1644,13 +1622,13 @@
         <v>43</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:1024" ht="38.25" x14ac:dyDescent="0.2">
@@ -1661,13 +1639,13 @@
         <v>46</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:1024" x14ac:dyDescent="0.2">
@@ -1678,13 +1656,13 @@
         <v>41</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
@@ -1695,13 +1673,13 @@
         <v>49</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
@@ -1712,13 +1690,13 @@
         <v>43</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
@@ -1729,13 +1707,13 @@
         <v>49</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:1024" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1746,13 +1724,13 @@
         <v>53</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="32" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
@@ -1763,19 +1741,19 @@
         <v>55</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F32" s="9"/>
     </row>
     <row r="33" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A33" s="23" t="s">
-        <v>56</v>
+      <c r="A33" s="1" t="s">
+        <v>209</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>12</v>
@@ -1792,58 +1770,58 @@
     </row>
     <row r="34" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="35" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="36" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="C36" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="C37" s="1">
         <v>10</v>
@@ -1863,7 +1841,7 @@
     </row>
     <row r="39" spans="1:1024" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -1871,146 +1849,146 @@
     </row>
     <row r="40" spans="1:1024" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B40" s="8" t="s">
-        <v>65</v>
-      </c>
       <c r="C40" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="41" spans="1:1024" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B41" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>167</v>
-      </c>
       <c r="D41" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="42" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="43" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="44" spans="1:1024" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="C44" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="45" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="46" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>46</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="47" spans="1:1024" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B47" s="8" t="s">
-        <v>74</v>
-      </c>
       <c r="C47" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="48" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="C48" s="1">
         <v>7</v>
@@ -2030,7 +2008,7 @@
     </row>
     <row r="50" spans="1:1024" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
@@ -2038,95 +2016,95 @@
     </row>
     <row r="51" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="52" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>43</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="53" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B53" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B53" s="8" t="s">
-        <v>79</v>
-      </c>
       <c r="C53" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="54" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>43</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="55" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>43</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="56" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="C56" s="1">
         <v>10</v>
@@ -2146,7 +2124,7 @@
     </row>
     <row r="58" spans="1:1024" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
@@ -2154,44 +2132,44 @@
     </row>
     <row r="59" spans="1:1024" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="C59" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="60" spans="1:1024" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="C60" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="61" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="C61" s="1">
         <v>9</v>
@@ -2211,7 +2189,7 @@
     </row>
     <row r="63" spans="1:1024" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
@@ -2219,78 +2197,78 @@
     </row>
     <row r="64" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="65" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="66" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="67" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="68" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="C68" s="1">
         <v>8</v>
@@ -2310,7 +2288,7 @@
     </row>
     <row r="70" spans="1:1024" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
@@ -2318,78 +2296,78 @@
     </row>
     <row r="71" spans="1:1024" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B71" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="72" spans="1:1024" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B72" s="8" t="s">
         <v>49</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="73" spans="1:1024" ht="280.5" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B73" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B73" s="8" t="s">
-        <v>96</v>
-      </c>
       <c r="C73" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="D73" s="1" t="s">
-        <v>195</v>
-      </c>
       <c r="E73" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="74" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B74" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="B74" s="8" t="s">
-        <v>98</v>
-      </c>
       <c r="C74" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="75" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="C75" s="15">
         <v>0.91649999999999998</v>
@@ -2403,10 +2381,10 @@
     </row>
     <row r="76" spans="1:1024" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B76" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C76" s="16">
         <f>C118/C116</f>
@@ -2423,27 +2401,27 @@
     </row>
     <row r="77" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A77" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B77" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="B77" s="8" t="s">
-        <v>103</v>
-      </c>
       <c r="C77" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="78" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="C78" s="1">
         <v>9</v>
@@ -2462,7 +2440,7 @@
     </row>
     <row r="80" spans="1:1024" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
@@ -2470,7 +2448,7 @@
     </row>
     <row r="81" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A81" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B81" s="8" t="s">
         <v>12</v>
@@ -2490,27 +2468,27 @@
     </row>
     <row r="82" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A82" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="83" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C83" s="1">
         <v>8</v>
@@ -2530,7 +2508,7 @@
     </row>
     <row r="85" spans="1:1024" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
@@ -2538,146 +2516,146 @@
     </row>
     <row r="86" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="87" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>111</v>
+        <v>211</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="88" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>86</v>
+        <v>210</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="89" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>86</v>
+        <v>210</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="90" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>86</v>
+        <v>210</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="91" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B91" s="23" t="s">
-        <v>86</v>
+        <v>113</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>210</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="92" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>86</v>
+        <v>210</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="93" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>86</v>
+        <v>210</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="94" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C94" s="1">
         <v>9</v>
@@ -2696,7 +2674,7 @@
     </row>
     <row r="96" spans="1:1024" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
@@ -2704,78 +2682,78 @@
     </row>
     <row r="97" spans="1:1024" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="98" spans="1:1024" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B98" s="8" t="s">
         <v>49</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="99" spans="1:1024" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B99" s="8" t="s">
         <v>37</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="100" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B100" s="8" t="s">
         <v>37</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="101" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B101" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="C101" s="1">
         <v>9</v>
@@ -2795,7 +2773,7 @@
     </row>
     <row r="105" spans="1:1024" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B105" s="5"/>
       <c r="C105" s="5"/>
@@ -2803,7 +2781,7 @@
     </row>
     <row r="106" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>12</v>
@@ -2820,7 +2798,7 @@
     </row>
     <row r="107" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>12</v>
@@ -2837,7 +2815,7 @@
     </row>
     <row r="108" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>12</v>
@@ -2854,7 +2832,7 @@
     </row>
     <row r="109" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>12</v>
@@ -2871,7 +2849,7 @@
     </row>
     <row r="110" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>12</v>
@@ -2888,7 +2866,7 @@
     </row>
     <row r="111" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>12</v>
@@ -2905,41 +2883,41 @@
     </row>
     <row r="112" spans="1:1024" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="113" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="114" spans="1:1024" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A114" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B114" s="5"/>
       <c r="C114" s="5"/>
@@ -2947,7 +2925,7 @@
     </row>
     <row r="115" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>12</v>
@@ -2964,7 +2942,7 @@
     </row>
     <row r="116" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>12</v>
@@ -2981,7 +2959,7 @@
     </row>
     <row r="117" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>12</v>
@@ -2998,7 +2976,7 @@
     </row>
     <row r="118" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>12</v>
@@ -3015,7 +2993,7 @@
     </row>
     <row r="119" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>12</v>
@@ -3032,7 +3010,7 @@
     </row>
     <row r="120" spans="1:1024" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B120" s="5"/>
       <c r="C120" s="5"/>
@@ -3040,10 +3018,10 @@
     </row>
     <row r="121" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B121" s="23" t="s">
-        <v>210</v>
+        <v>138</v>
+      </c>
+      <c r="B121" t="s">
+        <v>208</v>
       </c>
       <c r="C121" s="1">
         <v>132</v>
@@ -3052,15 +3030,15 @@
         <v>91</v>
       </c>
       <c r="E121" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="122" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B122" s="23" t="s">
-        <v>210</v>
+        <v>139</v>
+      </c>
+      <c r="B122" t="s">
+        <v>208</v>
       </c>
       <c r="C122" s="1">
         <v>63</v>
@@ -3069,15 +3047,15 @@
         <v>27</v>
       </c>
       <c r="E122" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="123" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B123" s="23" t="s">
-        <v>210</v>
+        <v>140</v>
+      </c>
+      <c r="B123" t="s">
+        <v>208</v>
       </c>
       <c r="C123" s="1">
         <v>19</v>
@@ -3086,15 +3064,15 @@
         <v>22</v>
       </c>
       <c r="E123" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="124" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B124" s="23" t="s">
-        <v>210</v>
+        <v>141</v>
+      </c>
+      <c r="B124" t="s">
+        <v>208</v>
       </c>
       <c r="C124" s="1">
         <v>10</v>
@@ -3103,15 +3081,15 @@
         <v>1</v>
       </c>
       <c r="E124" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="125" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B125" s="23" t="s">
-        <v>210</v>
+        <v>142</v>
+      </c>
+      <c r="B125" t="s">
+        <v>208</v>
       </c>
       <c r="C125" s="1">
         <v>215</v>
@@ -3120,7 +3098,7 @@
         <v>3</v>
       </c>
       <c r="E125" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>